<commit_message>
finish project (error correction)
</commit_message>
<xml_diff>
--- a/ExcelFile.xlsx
+++ b/ExcelFile.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Organization</t>
   </si>
@@ -36,6 +36,18 @@
   </si>
   <si>
     <t>2025</t>
+  </si>
+  <si>
+    <t>SBY</t>
+  </si>
+  <si>
+    <t>2024</t>
+  </si>
+  <si>
+    <t>ZSY</t>
+  </si>
+  <si>
+    <t>30</t>
   </si>
 </sst>
 </file>
@@ -80,7 +92,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -114,6 +126,34 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>